<commit_message>
Update build Manually. Add a colon in trap card data.
</commit_message>
<xml_diff>
--- a/sheet/TrapCardData.xlsx
+++ b/sheet/TrapCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6D1988-5C4A-4139-B889-5359A2B73D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33367AD4-5E20-4A0F-82E4-9E0C4AB8BA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,10 +195,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>被弃置时：选弃牌堆1张怪物牌送墓</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Teleporter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -225,6 +221,10 @@
   </si>
   <si>
     <t>Tomb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被弃置时：选弃牌堆1张怪物牌送墓。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -611,7 +611,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -645,7 +645,7 @@
     </row>
     <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -654,10 +654,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -794,7 +794,7 @@
         <v>37</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -812,7 +812,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -850,7 +850,7 @@
         <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -865,10 +865,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="4"/>
     </row>

</xml_diff>

<commit_message>
Update trap cards. Update preset decks to match new card names.
</commit_message>
<xml_diff>
--- a/sheet/TrapCardData.xlsx
+++ b/sheet/TrapCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76525CC-EA46-4885-8E91-F3B0A0030617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0848C6-4AF3-4065-B349-F964CC37AA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="3255" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,51 +193,52 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开战时，触发：本牌所在槽位和对位槽位的所有怪物牌点数变为1。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时，触发：如果本牌所在槽位和对位槽位的怪物牌合计数量不小于本牌点数，则将那些怪物牌全部消灭，然后消灭本牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时，触发：横置本牌，然后本牌所在槽位和对位槽位中所有其他牌点数减1。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时，触发：横置本牌所在槽位和对位槽位中所有牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本牌所在行列的槽位新增怪物牌时，触发：那张怪物牌点数减2，然后本牌点数减1。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时，触发：如果本牌点数大于1，则将本牌移动到相邻槽位中而不是送墓，然后使本牌和那个槽位中所有其他牌点数减1。&lt;br&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开战时，触发：如果本牌所在槽位和对位槽位的怪物牌合计数量大于1，则将那些怪物牌洗回主牌堆，然后消灭本牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点数降低时，触发：本牌所在槽位和相邻槽位的所有牌点数减1，然后消灭本牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有牌进入本牌所在槽位时，触发：本牌所在槽位和对位槽位中所有牌点数减1，然后消灭本牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时，触发：选本牌所在行或列，其中的所有牌点数减1。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时，触发：移动到1个相邻槽位，然后点数减1，本牌点数因此降至0时，消灭本牌所在槽位或对位槽位中的1张其他牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时，触发：将本牌移动到对位槽位，同槽位中有怪物牌时，选其中1张一起移动到对位槽位。</t>
+    <t>开战时，触发：同房间所有怪物牌点数变为1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时，触发：如果同房间怪物牌合计数量不小于本牌点数，消灭那些怪物牌，然后消灭本牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时，触发：横置本牌，然后同房间内所有其他牌点数减1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时，触发：横置同房间内所有牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同房间内怪物牌移入或移出时，触发：那张怪物牌点数减2，然后本牌点数减1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时，触发：如果本牌点数大于1，则将本牌移动到相邻房间中而不是送墓，然后使本牌和目标房间中所有其他牌点数减1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开战时，触发：如果同房间怪物牌合计数量大于1，则将那些怪物牌移入其他房间的同侧，然后消灭本牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点数降低时，触发：同房间所有牌点数减1，然后消灭本牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同房间内牌移入或移出时，触发：同房间内所有牌点数减1，然后消灭本牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时，触发：选1个相邻房间，使其中的所有牌点数减1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：移动1格，然后点数减1。&lt;br&gt;
+点数为0时，触发：消灭同房间1张其他牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时，触发：选同侧至多1张怪物牌，与本牌一起移动到对侧。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -623,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>